<commit_message>
Import staff data on EF.
</commit_message>
<xml_diff>
--- a/Docs/WSC2015_TP09_resources/WSC2015_TP09_resources_session-1/marathon-skills-2015-staff-import.xlsx
+++ b/Docs/WSC2015_TP09_resources/WSC2015_TP09_resources_session-1/marathon-skills-2015-staff-import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Staff" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="end_of_york">Timesheet!$F$35</definedName>
     <definedName name="positions">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1738,10 +1738,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1806,7 +1806,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1837,7 +1837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1856,23 +1856,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1880,8 +1880,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Денежный" xfId="1" builtinId="4"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1897,9 +1897,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1937,7 +1937,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2009,7 +2009,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>

</xml_diff>